<commit_message>
Falta só alertar o usuário quando ele colocar um valor indevido
</commit_message>
<xml_diff>
--- a/Erros.xlsx
+++ b/Erros.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\code\Catarata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CF05A9-1E99-47F6-9BA0-51C11104E9C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551F441D-7026-4D52-822E-53BD25655CF0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -40,10 +40,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,7 +101,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -146,7 +143,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -178,27 +175,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,24 +209,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D15" sqref="A2:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +419,19 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>